<commit_message>
encoded years for course categories
</commit_message>
<xml_diff>
--- a/sy2_data.xlsx
+++ b/sy2_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI62"/>
+  <dimension ref="A1:AJ62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,55 +556,60 @@
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
+          <t>encoded_year_taken</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
           <t>encoded_days</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Abbreviated Course Name</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>time_periods</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>duration_hours</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>total_duration_hours</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>course_classtype</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>ws_groups</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>no_of_agg_ws_groups</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>aggregated_ws_groups</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>sem1_pattern_one_hot</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>sem2_pattern_one_hot</t>
         </is>
@@ -717,41 +722,46 @@
       <c r="X2" t="n">
         <v>132</v>
       </c>
-      <c r="Y2" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA2" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA2" t="inlineStr">
+      <c r="AB2" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB2" t="n">
+      <c r="AC2" t="n">
         <v>1</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AD2" t="n">
         <v>5</v>
       </c>
-      <c r="AD2" t="inlineStr">
+      <c r="AE2" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE2" t="inlineStr"/>
-      <c r="AF2" t="n">
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="n">
         <v>9</v>
       </c>
-      <c r="AG2" t="inlineStr"/>
-      <c r="AH2" t="inlineStr">
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI2" t="inlineStr">
+      <c r="AJ2" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -864,41 +874,46 @@
       <c r="X3" t="n">
         <v>132</v>
       </c>
-      <c r="Y3" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z3" t="inlineStr">
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA3" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA3" t="inlineStr">
+      <c r="AB3" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB3" t="n">
+      <c r="AC3" t="n">
         <v>1</v>
       </c>
-      <c r="AC3" t="n">
+      <c r="AD3" t="n">
         <v>5</v>
       </c>
-      <c r="AD3" t="inlineStr">
+      <c r="AE3" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="n">
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="n">
         <v>9</v>
       </c>
-      <c r="AG3" t="inlineStr"/>
-      <c r="AH3" t="inlineStr">
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI3" t="inlineStr">
+      <c r="AJ3" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -1011,41 +1026,46 @@
       <c r="X4" t="n">
         <v>132</v>
       </c>
-      <c r="Y4" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z4" t="inlineStr">
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA4" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA4" t="inlineStr">
+      <c r="AB4" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB4" t="n">
+      <c r="AC4" t="n">
         <v>1</v>
       </c>
-      <c r="AC4" t="n">
+      <c r="AD4" t="n">
         <v>5</v>
       </c>
-      <c r="AD4" t="inlineStr">
+      <c r="AE4" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE4" t="inlineStr"/>
-      <c r="AF4" t="n">
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="n">
         <v>9</v>
       </c>
-      <c r="AG4" t="inlineStr"/>
-      <c r="AH4" t="inlineStr">
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI4" t="inlineStr">
+      <c r="AJ4" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -1158,41 +1178,46 @@
       <c r="X5" t="n">
         <v>132</v>
       </c>
-      <c r="Y5" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z5" t="inlineStr">
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA5" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA5" t="inlineStr">
+      <c r="AB5" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB5" t="n">
+      <c r="AC5" t="n">
         <v>1</v>
       </c>
-      <c r="AC5" t="n">
+      <c r="AD5" t="n">
         <v>5</v>
       </c>
-      <c r="AD5" t="inlineStr">
+      <c r="AE5" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE5" t="inlineStr"/>
-      <c r="AF5" t="n">
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="n">
         <v>9</v>
       </c>
-      <c r="AG5" t="inlineStr"/>
-      <c r="AH5" t="inlineStr">
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI5" t="inlineStr">
+      <c r="AJ5" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -1305,41 +1330,46 @@
       <c r="X6" t="n">
         <v>132</v>
       </c>
-      <c r="Y6" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z6" t="inlineStr">
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA6" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA6" t="inlineStr">
+      <c r="AB6" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB6" t="n">
+      <c r="AC6" t="n">
         <v>1</v>
       </c>
-      <c r="AC6" t="n">
+      <c r="AD6" t="n">
         <v>5</v>
       </c>
-      <c r="AD6" t="inlineStr">
+      <c r="AE6" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE6" t="inlineStr"/>
-      <c r="AF6" t="n">
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="n">
         <v>9</v>
       </c>
-      <c r="AG6" t="inlineStr"/>
-      <c r="AH6" t="inlineStr">
+      <c r="AH6" t="inlineStr"/>
+      <c r="AI6" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI6" t="inlineStr">
+      <c r="AJ6" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -1452,41 +1482,46 @@
       <c r="X7" t="n">
         <v>132</v>
       </c>
-      <c r="Y7" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z7" t="inlineStr">
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z7" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA7" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA7" t="inlineStr">
+      <c r="AB7" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB7" t="n">
+      <c r="AC7" t="n">
         <v>1</v>
       </c>
-      <c r="AC7" t="n">
+      <c r="AD7" t="n">
         <v>5</v>
       </c>
-      <c r="AD7" t="inlineStr">
+      <c r="AE7" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE7" t="inlineStr"/>
-      <c r="AF7" t="n">
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="n">
         <v>9</v>
       </c>
-      <c r="AG7" t="inlineStr"/>
-      <c r="AH7" t="inlineStr">
+      <c r="AH7" t="inlineStr"/>
+      <c r="AI7" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI7" t="inlineStr">
+      <c r="AJ7" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -1599,41 +1634,46 @@
       <c r="X8" t="n">
         <v>132</v>
       </c>
-      <c r="Y8" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z8" t="inlineStr">
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z8" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA8" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA8" t="inlineStr">
+      <c r="AB8" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB8" t="n">
+      <c r="AC8" t="n">
         <v>1</v>
       </c>
-      <c r="AC8" t="n">
+      <c r="AD8" t="n">
         <v>5</v>
       </c>
-      <c r="AD8" t="inlineStr">
+      <c r="AE8" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE8" t="inlineStr"/>
-      <c r="AF8" t="n">
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="n">
         <v>9</v>
       </c>
-      <c r="AG8" t="inlineStr"/>
-      <c r="AH8" t="inlineStr">
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI8" t="inlineStr">
+      <c r="AJ8" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -1746,41 +1786,46 @@
       <c r="X9" t="n">
         <v>132</v>
       </c>
-      <c r="Y9" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z9" t="inlineStr">
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z9" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA9" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA9" t="inlineStr">
+      <c r="AB9" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB9" t="n">
+      <c r="AC9" t="n">
         <v>1</v>
       </c>
-      <c r="AC9" t="n">
+      <c r="AD9" t="n">
         <v>5</v>
       </c>
-      <c r="AD9" t="inlineStr">
+      <c r="AE9" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE9" t="inlineStr"/>
-      <c r="AF9" t="n">
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="n">
         <v>9</v>
       </c>
-      <c r="AG9" t="inlineStr"/>
-      <c r="AH9" t="inlineStr">
+      <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI9" t="inlineStr">
+      <c r="AJ9" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -1893,41 +1938,46 @@
       <c r="X10" t="n">
         <v>132</v>
       </c>
-      <c r="Y10" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z10" t="inlineStr">
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z10" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA10" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA10" t="inlineStr">
+      <c r="AB10" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB10" t="n">
+      <c r="AC10" t="n">
         <v>1</v>
       </c>
-      <c r="AC10" t="n">
+      <c r="AD10" t="n">
         <v>5</v>
       </c>
-      <c r="AD10" t="inlineStr">
+      <c r="AE10" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE10" t="inlineStr"/>
-      <c r="AF10" t="n">
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="n">
         <v>9</v>
       </c>
-      <c r="AG10" t="inlineStr"/>
-      <c r="AH10" t="inlineStr">
+      <c r="AH10" t="inlineStr"/>
+      <c r="AI10" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI10" t="inlineStr">
+      <c r="AJ10" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -2040,41 +2090,46 @@
       <c r="X11" t="n">
         <v>132</v>
       </c>
-      <c r="Y11" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z11" t="inlineStr">
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z11" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA11" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA11" t="inlineStr">
+      <c r="AB11" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB11" t="n">
+      <c r="AC11" t="n">
         <v>1</v>
       </c>
-      <c r="AC11" t="n">
+      <c r="AD11" t="n">
         <v>5</v>
       </c>
-      <c r="AD11" t="inlineStr">
+      <c r="AE11" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE11" t="inlineStr"/>
-      <c r="AF11" t="n">
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="n">
         <v>9</v>
       </c>
-      <c r="AG11" t="inlineStr"/>
-      <c r="AH11" t="inlineStr">
+      <c r="AH11" t="inlineStr"/>
+      <c r="AI11" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI11" t="inlineStr">
+      <c r="AJ11" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -2187,41 +2242,46 @@
       <c r="X12" t="n">
         <v>132</v>
       </c>
-      <c r="Y12" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z12" t="inlineStr">
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA12" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA12" t="inlineStr">
+      <c r="AB12" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB12" t="n">
+      <c r="AC12" t="n">
         <v>1</v>
       </c>
-      <c r="AC12" t="n">
+      <c r="AD12" t="n">
         <v>5</v>
       </c>
-      <c r="AD12" t="inlineStr">
+      <c r="AE12" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE12" t="inlineStr"/>
-      <c r="AF12" t="n">
+      <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="n">
         <v>9</v>
       </c>
-      <c r="AG12" t="inlineStr"/>
-      <c r="AH12" t="inlineStr">
+      <c r="AH12" t="inlineStr"/>
+      <c r="AI12" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI12" t="inlineStr">
+      <c r="AJ12" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -2334,41 +2394,46 @@
       <c r="X13" t="n">
         <v>132</v>
       </c>
-      <c r="Y13" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z13" t="inlineStr">
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z13" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA13" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA13" t="inlineStr">
+      <c r="AB13" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB13" t="n">
+      <c r="AC13" t="n">
         <v>1</v>
       </c>
-      <c r="AC13" t="n">
+      <c r="AD13" t="n">
         <v>5</v>
       </c>
-      <c r="AD13" t="inlineStr">
+      <c r="AE13" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE13" t="inlineStr"/>
-      <c r="AF13" t="n">
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="n">
         <v>9</v>
       </c>
-      <c r="AG13" t="inlineStr"/>
-      <c r="AH13" t="inlineStr">
+      <c r="AH13" t="inlineStr"/>
+      <c r="AI13" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI13" t="inlineStr">
+      <c r="AJ13" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -2481,41 +2546,46 @@
       <c r="X14" t="n">
         <v>132</v>
       </c>
-      <c r="Y14" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z14" t="inlineStr">
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA14" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA14" t="inlineStr">
+      <c r="AB14" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB14" t="n">
+      <c r="AC14" t="n">
         <v>1</v>
       </c>
-      <c r="AC14" t="n">
+      <c r="AD14" t="n">
         <v>5</v>
       </c>
-      <c r="AD14" t="inlineStr">
+      <c r="AE14" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE14" t="inlineStr"/>
-      <c r="AF14" t="n">
+      <c r="AF14" t="inlineStr"/>
+      <c r="AG14" t="n">
         <v>9</v>
       </c>
-      <c r="AG14" t="inlineStr"/>
-      <c r="AH14" t="inlineStr">
+      <c r="AH14" t="inlineStr"/>
+      <c r="AI14" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI14" t="inlineStr">
+      <c r="AJ14" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -2628,41 +2698,46 @@
       <c r="X15" t="n">
         <v>132</v>
       </c>
-      <c r="Y15" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z15" t="inlineStr">
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z15" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA15" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA15" t="inlineStr">
+      <c r="AB15" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB15" t="n">
+      <c r="AC15" t="n">
         <v>1</v>
       </c>
-      <c r="AC15" t="n">
+      <c r="AD15" t="n">
         <v>5</v>
       </c>
-      <c r="AD15" t="inlineStr">
+      <c r="AE15" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE15" t="inlineStr"/>
-      <c r="AF15" t="n">
+      <c r="AF15" t="inlineStr"/>
+      <c r="AG15" t="n">
         <v>9</v>
       </c>
-      <c r="AG15" t="inlineStr"/>
-      <c r="AH15" t="inlineStr">
+      <c r="AH15" t="inlineStr"/>
+      <c r="AI15" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI15" t="inlineStr">
+      <c r="AJ15" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -2775,41 +2850,46 @@
       <c r="X16" t="n">
         <v>72</v>
       </c>
-      <c r="Y16" t="n">
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z16" t="n">
         <v>5</v>
       </c>
-      <c r="Z16" t="inlineStr">
+      <c r="AA16" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA16" t="inlineStr">
+      <c r="AB16" t="inlineStr">
         <is>
           <t>3, 4</t>
         </is>
       </c>
-      <c r="AB16" t="n">
+      <c r="AC16" t="n">
         <v>1</v>
       </c>
-      <c r="AC16" t="n">
+      <c r="AD16" t="n">
         <v>5</v>
       </c>
-      <c r="AD16" t="inlineStr">
+      <c r="AE16" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE16" t="inlineStr"/>
-      <c r="AF16" t="n">
+      <c r="AF16" t="inlineStr"/>
+      <c r="AG16" t="n">
         <v>5</v>
       </c>
-      <c r="AG16" t="inlineStr"/>
-      <c r="AH16" t="inlineStr">
+      <c r="AH16" t="inlineStr"/>
+      <c r="AI16" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI16" t="inlineStr">
+      <c r="AJ16" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -2922,41 +3002,46 @@
       <c r="X17" t="n">
         <v>72</v>
       </c>
-      <c r="Y17" t="n">
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z17" t="n">
         <v>5</v>
       </c>
-      <c r="Z17" t="inlineStr">
+      <c r="AA17" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA17" t="inlineStr">
+      <c r="AB17" t="inlineStr">
         <is>
           <t>3, 4</t>
         </is>
       </c>
-      <c r="AB17" t="n">
+      <c r="AC17" t="n">
         <v>1</v>
       </c>
-      <c r="AC17" t="n">
+      <c r="AD17" t="n">
         <v>5</v>
       </c>
-      <c r="AD17" t="inlineStr">
+      <c r="AE17" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE17" t="inlineStr"/>
-      <c r="AF17" t="n">
+      <c r="AF17" t="inlineStr"/>
+      <c r="AG17" t="n">
         <v>5</v>
       </c>
-      <c r="AG17" t="inlineStr"/>
-      <c r="AH17" t="inlineStr">
+      <c r="AH17" t="inlineStr"/>
+      <c r="AI17" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI17" t="inlineStr">
+      <c r="AJ17" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -3069,41 +3154,46 @@
       <c r="X18" t="n">
         <v>72</v>
       </c>
-      <c r="Y18" t="n">
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z18" t="n">
         <v>5</v>
       </c>
-      <c r="Z18" t="inlineStr">
+      <c r="AA18" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA18" t="inlineStr">
+      <c r="AB18" t="inlineStr">
         <is>
           <t>3, 4</t>
         </is>
       </c>
-      <c r="AB18" t="n">
+      <c r="AC18" t="n">
         <v>1</v>
       </c>
-      <c r="AC18" t="n">
+      <c r="AD18" t="n">
         <v>5</v>
       </c>
-      <c r="AD18" t="inlineStr">
+      <c r="AE18" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE18" t="inlineStr"/>
-      <c r="AF18" t="n">
+      <c r="AF18" t="inlineStr"/>
+      <c r="AG18" t="n">
         <v>5</v>
       </c>
-      <c r="AG18" t="inlineStr"/>
-      <c r="AH18" t="inlineStr">
+      <c r="AH18" t="inlineStr"/>
+      <c r="AI18" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI18" t="inlineStr">
+      <c r="AJ18" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -3216,41 +3306,46 @@
       <c r="X19" t="n">
         <v>72</v>
       </c>
-      <c r="Y19" t="n">
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z19" t="n">
         <v>5</v>
       </c>
-      <c r="Z19" t="inlineStr">
+      <c r="AA19" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA19" t="inlineStr">
+      <c r="AB19" t="inlineStr">
         <is>
           <t>5, 6</t>
         </is>
       </c>
-      <c r="AB19" t="n">
+      <c r="AC19" t="n">
         <v>1</v>
       </c>
-      <c r="AC19" t="n">
+      <c r="AD19" t="n">
         <v>5</v>
       </c>
-      <c r="AD19" t="inlineStr">
+      <c r="AE19" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE19" t="inlineStr"/>
-      <c r="AF19" t="n">
+      <c r="AF19" t="inlineStr"/>
+      <c r="AG19" t="n">
         <v>5</v>
       </c>
-      <c r="AG19" t="inlineStr"/>
-      <c r="AH19" t="inlineStr">
+      <c r="AH19" t="inlineStr"/>
+      <c r="AI19" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI19" t="inlineStr">
+      <c r="AJ19" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -3363,41 +3458,46 @@
       <c r="X20" t="n">
         <v>72</v>
       </c>
-      <c r="Y20" t="n">
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z20" t="n">
         <v>5</v>
       </c>
-      <c r="Z20" t="inlineStr">
+      <c r="AA20" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA20" t="inlineStr">
+      <c r="AB20" t="inlineStr">
         <is>
           <t>5, 6</t>
         </is>
       </c>
-      <c r="AB20" t="n">
+      <c r="AC20" t="n">
         <v>1</v>
       </c>
-      <c r="AC20" t="n">
+      <c r="AD20" t="n">
         <v>5</v>
       </c>
-      <c r="AD20" t="inlineStr">
+      <c r="AE20" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE20" t="inlineStr"/>
-      <c r="AF20" t="n">
+      <c r="AF20" t="inlineStr"/>
+      <c r="AG20" t="n">
         <v>5</v>
       </c>
-      <c r="AG20" t="inlineStr"/>
-      <c r="AH20" t="inlineStr">
+      <c r="AH20" t="inlineStr"/>
+      <c r="AI20" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI20" t="inlineStr">
+      <c r="AJ20" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -3510,41 +3610,46 @@
       <c r="X21" t="n">
         <v>72</v>
       </c>
-      <c r="Y21" t="n">
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z21" t="n">
         <v>5</v>
       </c>
-      <c r="Z21" t="inlineStr">
+      <c r="AA21" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA21" t="inlineStr">
+      <c r="AB21" t="inlineStr">
         <is>
           <t>5, 6</t>
         </is>
       </c>
-      <c r="AB21" t="n">
+      <c r="AC21" t="n">
         <v>1</v>
       </c>
-      <c r="AC21" t="n">
+      <c r="AD21" t="n">
         <v>5</v>
       </c>
-      <c r="AD21" t="inlineStr">
+      <c r="AE21" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE21" t="inlineStr"/>
-      <c r="AF21" t="n">
+      <c r="AF21" t="inlineStr"/>
+      <c r="AG21" t="n">
         <v>5</v>
       </c>
-      <c r="AG21" t="inlineStr"/>
-      <c r="AH21" t="inlineStr">
+      <c r="AH21" t="inlineStr"/>
+      <c r="AI21" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI21" t="inlineStr">
+      <c r="AJ21" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -3657,41 +3762,46 @@
       <c r="X22" t="n">
         <v>72</v>
       </c>
-      <c r="Y22" t="n">
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z22" t="n">
         <v>5</v>
       </c>
-      <c r="Z22" t="inlineStr">
+      <c r="AA22" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA22" t="inlineStr">
+      <c r="AB22" t="inlineStr">
         <is>
           <t>3, 4</t>
         </is>
       </c>
-      <c r="AB22" t="n">
+      <c r="AC22" t="n">
         <v>1</v>
       </c>
-      <c r="AC22" t="n">
+      <c r="AD22" t="n">
         <v>5</v>
       </c>
-      <c r="AD22" t="inlineStr">
+      <c r="AE22" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE22" t="inlineStr"/>
-      <c r="AF22" t="n">
+      <c r="AF22" t="inlineStr"/>
+      <c r="AG22" t="n">
         <v>5</v>
       </c>
-      <c r="AG22" t="inlineStr"/>
-      <c r="AH22" t="inlineStr">
+      <c r="AH22" t="inlineStr"/>
+      <c r="AI22" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI22" t="inlineStr">
+      <c r="AJ22" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -3804,41 +3914,46 @@
       <c r="X23" t="n">
         <v>72</v>
       </c>
-      <c r="Y23" t="n">
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z23" t="n">
         <v>5</v>
       </c>
-      <c r="Z23" t="inlineStr">
+      <c r="AA23" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA23" t="inlineStr">
+      <c r="AB23" t="inlineStr">
         <is>
           <t>5, 6</t>
         </is>
       </c>
-      <c r="AB23" t="n">
+      <c r="AC23" t="n">
         <v>1</v>
       </c>
-      <c r="AC23" t="n">
+      <c r="AD23" t="n">
         <v>5</v>
       </c>
-      <c r="AD23" t="inlineStr">
+      <c r="AE23" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE23" t="inlineStr"/>
-      <c r="AF23" t="n">
+      <c r="AF23" t="inlineStr"/>
+      <c r="AG23" t="n">
         <v>5</v>
       </c>
-      <c r="AG23" t="inlineStr"/>
-      <c r="AH23" t="inlineStr">
+      <c r="AH23" t="inlineStr"/>
+      <c r="AI23" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI23" t="inlineStr">
+      <c r="AJ23" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -3951,41 +4066,46 @@
       <c r="X24" t="n">
         <v>132</v>
       </c>
-      <c r="Y24" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z24" t="inlineStr">
+      <c r="Y24" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z24" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA24" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA24" t="inlineStr">
+      <c r="AB24" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB24" t="n">
+      <c r="AC24" t="n">
         <v>1</v>
       </c>
-      <c r="AC24" t="n">
+      <c r="AD24" t="n">
         <v>5</v>
       </c>
-      <c r="AD24" t="inlineStr">
+      <c r="AE24" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE24" t="inlineStr"/>
-      <c r="AF24" t="n">
+      <c r="AF24" t="inlineStr"/>
+      <c r="AG24" t="n">
         <v>9</v>
       </c>
-      <c r="AG24" t="inlineStr"/>
-      <c r="AH24" t="inlineStr">
+      <c r="AH24" t="inlineStr"/>
+      <c r="AI24" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI24" t="inlineStr">
+      <c r="AJ24" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -4098,41 +4218,46 @@
       <c r="X25" t="n">
         <v>60</v>
       </c>
-      <c r="Y25" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z25" t="inlineStr">
+      <c r="Y25" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z25" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA25" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA25" t="inlineStr">
+      <c r="AB25" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB25" t="n">
+      <c r="AC25" t="n">
         <v>1</v>
       </c>
-      <c r="AC25" t="n">
+      <c r="AD25" t="n">
         <v>5</v>
       </c>
-      <c r="AD25" t="inlineStr">
+      <c r="AE25" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE25" t="inlineStr"/>
-      <c r="AF25" t="n">
+      <c r="AF25" t="inlineStr"/>
+      <c r="AG25" t="n">
         <v>9</v>
       </c>
-      <c r="AG25" t="inlineStr"/>
-      <c r="AH25" t="inlineStr">
+      <c r="AH25" t="inlineStr"/>
+      <c r="AI25" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI25" t="inlineStr">
+      <c r="AJ25" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -4241,41 +4366,46 @@
       <c r="X26" t="n">
         <v>132</v>
       </c>
-      <c r="Y26" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z26" t="inlineStr">
+      <c r="Y26" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z26" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA26" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA26" t="inlineStr">
+      <c r="AB26" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB26" t="n">
+      <c r="AC26" t="n">
         <v>1</v>
       </c>
-      <c r="AC26" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD26" t="inlineStr">
+      <c r="AD26" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE26" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE26" t="inlineStr"/>
-      <c r="AF26" t="n">
+      <c r="AF26" t="inlineStr"/>
+      <c r="AG26" t="n">
         <v>14</v>
       </c>
-      <c r="AG26" t="inlineStr"/>
-      <c r="AH26" t="inlineStr">
+      <c r="AH26" t="inlineStr"/>
+      <c r="AI26" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI26" t="inlineStr">
+      <c r="AJ26" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -4384,41 +4514,46 @@
       <c r="X27" t="n">
         <v>132</v>
       </c>
-      <c r="Y27" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z27" t="inlineStr">
+      <c r="Y27" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z27" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA27" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA27" t="inlineStr">
+      <c r="AB27" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB27" t="n">
+      <c r="AC27" t="n">
         <v>1</v>
       </c>
-      <c r="AC27" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD27" t="inlineStr">
+      <c r="AD27" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE27" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE27" t="inlineStr"/>
-      <c r="AF27" t="n">
+      <c r="AF27" t="inlineStr"/>
+      <c r="AG27" t="n">
         <v>14</v>
       </c>
-      <c r="AG27" t="inlineStr"/>
-      <c r="AH27" t="inlineStr">
+      <c r="AH27" t="inlineStr"/>
+      <c r="AI27" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI27" t="inlineStr">
+      <c r="AJ27" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -4527,41 +4662,46 @@
       <c r="X28" t="n">
         <v>132</v>
       </c>
-      <c r="Y28" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z28" t="inlineStr">
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z28" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA28" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA28" t="inlineStr">
+      <c r="AB28" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB28" t="n">
+      <c r="AC28" t="n">
         <v>1</v>
       </c>
-      <c r="AC28" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD28" t="inlineStr">
+      <c r="AD28" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE28" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE28" t="inlineStr"/>
-      <c r="AF28" t="n">
+      <c r="AF28" t="inlineStr"/>
+      <c r="AG28" t="n">
         <v>14</v>
       </c>
-      <c r="AG28" t="inlineStr"/>
-      <c r="AH28" t="inlineStr">
+      <c r="AH28" t="inlineStr"/>
+      <c r="AI28" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI28" t="inlineStr">
+      <c r="AJ28" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -4670,41 +4810,46 @@
       <c r="X29" t="n">
         <v>132</v>
       </c>
-      <c r="Y29" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z29" t="inlineStr">
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z29" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA29" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA29" t="inlineStr">
+      <c r="AB29" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB29" t="n">
+      <c r="AC29" t="n">
         <v>1</v>
       </c>
-      <c r="AC29" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD29" t="inlineStr">
+      <c r="AD29" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE29" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE29" t="inlineStr"/>
-      <c r="AF29" t="n">
+      <c r="AF29" t="inlineStr"/>
+      <c r="AG29" t="n">
         <v>14</v>
       </c>
-      <c r="AG29" t="inlineStr"/>
-      <c r="AH29" t="inlineStr">
+      <c r="AH29" t="inlineStr"/>
+      <c r="AI29" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI29" t="inlineStr">
+      <c r="AJ29" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -4813,41 +4958,46 @@
       <c r="X30" t="n">
         <v>132</v>
       </c>
-      <c r="Y30" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z30" t="inlineStr">
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z30" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA30" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA30" t="inlineStr">
+      <c r="AB30" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB30" t="n">
+      <c r="AC30" t="n">
         <v>1</v>
       </c>
-      <c r="AC30" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD30" t="inlineStr">
+      <c r="AD30" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE30" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE30" t="inlineStr"/>
-      <c r="AF30" t="n">
+      <c r="AF30" t="inlineStr"/>
+      <c r="AG30" t="n">
         <v>14</v>
       </c>
-      <c r="AG30" t="inlineStr"/>
-      <c r="AH30" t="inlineStr">
+      <c r="AH30" t="inlineStr"/>
+      <c r="AI30" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI30" t="inlineStr">
+      <c r="AJ30" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -4956,41 +5106,46 @@
       <c r="X31" t="n">
         <v>132</v>
       </c>
-      <c r="Y31" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z31" t="inlineStr">
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z31" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA31" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA31" t="inlineStr">
+      <c r="AB31" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB31" t="n">
+      <c r="AC31" t="n">
         <v>1</v>
       </c>
-      <c r="AC31" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD31" t="inlineStr">
+      <c r="AD31" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE31" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE31" t="inlineStr"/>
-      <c r="AF31" t="n">
+      <c r="AF31" t="inlineStr"/>
+      <c r="AG31" t="n">
         <v>14</v>
       </c>
-      <c r="AG31" t="inlineStr"/>
-      <c r="AH31" t="inlineStr">
+      <c r="AH31" t="inlineStr"/>
+      <c r="AI31" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI31" t="inlineStr">
+      <c r="AJ31" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -5099,41 +5254,46 @@
       <c r="X32" t="n">
         <v>132</v>
       </c>
-      <c r="Y32" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z32" t="inlineStr">
+      <c r="Y32" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z32" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA32" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA32" t="inlineStr">
+      <c r="AB32" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB32" t="n">
+      <c r="AC32" t="n">
         <v>1</v>
       </c>
-      <c r="AC32" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD32" t="inlineStr">
+      <c r="AD32" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE32" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE32" t="inlineStr"/>
-      <c r="AF32" t="n">
+      <c r="AF32" t="inlineStr"/>
+      <c r="AG32" t="n">
         <v>14</v>
       </c>
-      <c r="AG32" t="inlineStr"/>
-      <c r="AH32" t="inlineStr">
+      <c r="AH32" t="inlineStr"/>
+      <c r="AI32" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI32" t="inlineStr">
+      <c r="AJ32" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -5242,41 +5402,46 @@
       <c r="X33" t="n">
         <v>101</v>
       </c>
-      <c r="Y33" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z33" t="inlineStr">
+      <c r="Y33" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z33" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA33" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA33" t="inlineStr">
+      <c r="AB33" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB33" t="n">
+      <c r="AC33" t="n">
         <v>1</v>
       </c>
-      <c r="AC33" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD33" t="inlineStr">
+      <c r="AD33" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE33" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE33" t="inlineStr"/>
-      <c r="AF33" t="n">
+      <c r="AF33" t="inlineStr"/>
+      <c r="AG33" t="n">
         <v>14</v>
       </c>
-      <c r="AG33" t="inlineStr"/>
-      <c r="AH33" t="inlineStr">
+      <c r="AH33" t="inlineStr"/>
+      <c r="AI33" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI33" t="inlineStr">
+      <c r="AJ33" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -5385,41 +5550,46 @@
       <c r="X34" t="n">
         <v>101</v>
       </c>
-      <c r="Y34" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z34" t="inlineStr">
+      <c r="Y34" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z34" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA34" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA34" t="inlineStr">
+      <c r="AB34" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB34" t="n">
+      <c r="AC34" t="n">
         <v>1</v>
       </c>
-      <c r="AC34" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD34" t="inlineStr">
+      <c r="AD34" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE34" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE34" t="inlineStr"/>
-      <c r="AF34" t="n">
+      <c r="AF34" t="inlineStr"/>
+      <c r="AG34" t="n">
         <v>14</v>
       </c>
-      <c r="AG34" t="inlineStr"/>
-      <c r="AH34" t="inlineStr">
+      <c r="AH34" t="inlineStr"/>
+      <c r="AI34" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI34" t="inlineStr">
+      <c r="AJ34" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -5528,41 +5698,46 @@
       <c r="X35" t="n">
         <v>101</v>
       </c>
-      <c r="Y35" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z35" t="inlineStr">
+      <c r="Y35" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z35" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA35" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA35" t="inlineStr">
+      <c r="AB35" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB35" t="n">
+      <c r="AC35" t="n">
         <v>1</v>
       </c>
-      <c r="AC35" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD35" t="inlineStr">
+      <c r="AD35" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE35" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE35" t="inlineStr"/>
-      <c r="AF35" t="n">
+      <c r="AF35" t="inlineStr"/>
+      <c r="AG35" t="n">
         <v>14</v>
       </c>
-      <c r="AG35" t="inlineStr"/>
-      <c r="AH35" t="inlineStr">
+      <c r="AH35" t="inlineStr"/>
+      <c r="AI35" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI35" t="inlineStr">
+      <c r="AJ35" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -5671,41 +5846,46 @@
       <c r="X36" t="n">
         <v>101</v>
       </c>
-      <c r="Y36" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z36" t="inlineStr">
+      <c r="Y36" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z36" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA36" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA36" t="inlineStr">
+      <c r="AB36" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB36" t="n">
+      <c r="AC36" t="n">
         <v>1</v>
       </c>
-      <c r="AC36" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD36" t="inlineStr">
+      <c r="AD36" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE36" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE36" t="inlineStr"/>
-      <c r="AF36" t="n">
+      <c r="AF36" t="inlineStr"/>
+      <c r="AG36" t="n">
         <v>14</v>
       </c>
-      <c r="AG36" t="inlineStr"/>
-      <c r="AH36" t="inlineStr">
+      <c r="AH36" t="inlineStr"/>
+      <c r="AI36" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI36" t="inlineStr">
+      <c r="AJ36" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -5814,41 +5994,46 @@
       <c r="X37" t="n">
         <v>101</v>
       </c>
-      <c r="Y37" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z37" t="inlineStr">
+      <c r="Y37" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z37" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA37" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA37" t="inlineStr">
+      <c r="AB37" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB37" t="n">
+      <c r="AC37" t="n">
         <v>1</v>
       </c>
-      <c r="AC37" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD37" t="inlineStr">
+      <c r="AD37" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE37" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE37" t="inlineStr"/>
-      <c r="AF37" t="n">
+      <c r="AF37" t="inlineStr"/>
+      <c r="AG37" t="n">
         <v>14</v>
       </c>
-      <c r="AG37" t="inlineStr"/>
-      <c r="AH37" t="inlineStr">
+      <c r="AH37" t="inlineStr"/>
+      <c r="AI37" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI37" t="inlineStr">
+      <c r="AJ37" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -5957,41 +6142,46 @@
       <c r="X38" t="n">
         <v>132</v>
       </c>
-      <c r="Y38" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z38" t="inlineStr">
+      <c r="Y38" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z38" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA38" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA38" t="inlineStr">
+      <c r="AB38" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB38" t="n">
+      <c r="AC38" t="n">
         <v>1</v>
       </c>
-      <c r="AC38" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD38" t="inlineStr">
+      <c r="AD38" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE38" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE38" t="inlineStr"/>
-      <c r="AF38" t="n">
+      <c r="AF38" t="inlineStr"/>
+      <c r="AG38" t="n">
         <v>13</v>
       </c>
-      <c r="AG38" t="inlineStr"/>
-      <c r="AH38" t="inlineStr">
+      <c r="AH38" t="inlineStr"/>
+      <c r="AI38" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI38" t="inlineStr">
+      <c r="AJ38" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -6100,41 +6290,46 @@
       <c r="X39" t="n">
         <v>132</v>
       </c>
-      <c r="Y39" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z39" t="inlineStr">
+      <c r="Y39" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z39" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA39" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA39" t="inlineStr">
+      <c r="AB39" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB39" t="n">
+      <c r="AC39" t="n">
         <v>1</v>
       </c>
-      <c r="AC39" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD39" t="inlineStr">
+      <c r="AD39" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE39" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE39" t="inlineStr"/>
-      <c r="AF39" t="n">
+      <c r="AF39" t="inlineStr"/>
+      <c r="AG39" t="n">
         <v>13</v>
       </c>
-      <c r="AG39" t="inlineStr"/>
-      <c r="AH39" t="inlineStr">
+      <c r="AH39" t="inlineStr"/>
+      <c r="AI39" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI39" t="inlineStr">
+      <c r="AJ39" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -6243,41 +6438,46 @@
       <c r="X40" t="n">
         <v>132</v>
       </c>
-      <c r="Y40" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z40" t="inlineStr">
+      <c r="Y40" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z40" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA40" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA40" t="inlineStr">
+      <c r="AB40" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB40" t="n">
+      <c r="AC40" t="n">
         <v>1</v>
       </c>
-      <c r="AC40" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD40" t="inlineStr">
+      <c r="AD40" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE40" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE40" t="inlineStr"/>
-      <c r="AF40" t="n">
+      <c r="AF40" t="inlineStr"/>
+      <c r="AG40" t="n">
         <v>13</v>
       </c>
-      <c r="AG40" t="inlineStr"/>
-      <c r="AH40" t="inlineStr">
+      <c r="AH40" t="inlineStr"/>
+      <c r="AI40" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI40" t="inlineStr">
+      <c r="AJ40" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -6386,41 +6586,46 @@
       <c r="X41" t="n">
         <v>132</v>
       </c>
-      <c r="Y41" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z41" t="inlineStr">
+      <c r="Y41" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z41" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA41" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA41" t="inlineStr">
+      <c r="AB41" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB41" t="n">
+      <c r="AC41" t="n">
         <v>1</v>
       </c>
-      <c r="AC41" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD41" t="inlineStr">
+      <c r="AD41" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE41" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE41" t="inlineStr"/>
-      <c r="AF41" t="n">
+      <c r="AF41" t="inlineStr"/>
+      <c r="AG41" t="n">
         <v>13</v>
       </c>
-      <c r="AG41" t="inlineStr"/>
-      <c r="AH41" t="inlineStr">
+      <c r="AH41" t="inlineStr"/>
+      <c r="AI41" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI41" t="inlineStr">
+      <c r="AJ41" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -6529,41 +6734,46 @@
       <c r="X42" t="n">
         <v>132</v>
       </c>
-      <c r="Y42" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z42" t="inlineStr">
+      <c r="Y42" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z42" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA42" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA42" t="inlineStr">
+      <c r="AB42" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB42" t="n">
+      <c r="AC42" t="n">
         <v>1</v>
       </c>
-      <c r="AC42" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD42" t="inlineStr">
+      <c r="AD42" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE42" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE42" t="inlineStr"/>
-      <c r="AF42" t="n">
+      <c r="AF42" t="inlineStr"/>
+      <c r="AG42" t="n">
         <v>13</v>
       </c>
-      <c r="AG42" t="inlineStr"/>
-      <c r="AH42" t="inlineStr">
+      <c r="AH42" t="inlineStr"/>
+      <c r="AI42" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI42" t="inlineStr">
+      <c r="AJ42" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -6672,41 +6882,46 @@
       <c r="X43" t="n">
         <v>132</v>
       </c>
-      <c r="Y43" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z43" t="inlineStr">
+      <c r="Y43" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z43" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA43" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA43" t="inlineStr">
+      <c r="AB43" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB43" t="n">
+      <c r="AC43" t="n">
         <v>1</v>
       </c>
-      <c r="AC43" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD43" t="inlineStr">
+      <c r="AD43" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE43" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE43" t="inlineStr"/>
-      <c r="AF43" t="n">
+      <c r="AF43" t="inlineStr"/>
+      <c r="AG43" t="n">
         <v>13</v>
       </c>
-      <c r="AG43" t="inlineStr"/>
-      <c r="AH43" t="inlineStr">
+      <c r="AH43" t="inlineStr"/>
+      <c r="AI43" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI43" t="inlineStr">
+      <c r="AJ43" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -6815,41 +7030,46 @@
       <c r="X44" t="n">
         <v>101</v>
       </c>
-      <c r="Y44" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z44" t="inlineStr">
+      <c r="Y44" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z44" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA44" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA44" t="inlineStr">
+      <c r="AB44" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB44" t="n">
+      <c r="AC44" t="n">
         <v>1</v>
       </c>
-      <c r="AC44" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD44" t="inlineStr">
+      <c r="AD44" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE44" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE44" t="inlineStr"/>
-      <c r="AF44" t="n">
+      <c r="AF44" t="inlineStr"/>
+      <c r="AG44" t="n">
         <v>13</v>
       </c>
-      <c r="AG44" t="inlineStr"/>
-      <c r="AH44" t="inlineStr">
+      <c r="AH44" t="inlineStr"/>
+      <c r="AI44" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI44" t="inlineStr">
+      <c r="AJ44" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -6958,41 +7178,46 @@
       <c r="X45" t="n">
         <v>101</v>
       </c>
-      <c r="Y45" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z45" t="inlineStr">
+      <c r="Y45" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z45" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA45" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA45" t="inlineStr">
+      <c r="AB45" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB45" t="n">
+      <c r="AC45" t="n">
         <v>1</v>
       </c>
-      <c r="AC45" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD45" t="inlineStr">
+      <c r="AD45" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE45" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE45" t="inlineStr"/>
-      <c r="AF45" t="n">
+      <c r="AF45" t="inlineStr"/>
+      <c r="AG45" t="n">
         <v>13</v>
       </c>
-      <c r="AG45" t="inlineStr"/>
-      <c r="AH45" t="inlineStr">
+      <c r="AH45" t="inlineStr"/>
+      <c r="AI45" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI45" t="inlineStr">
+      <c r="AJ45" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -7101,41 +7326,46 @@
       <c r="X46" t="n">
         <v>101</v>
       </c>
-      <c r="Y46" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z46" t="inlineStr">
+      <c r="Y46" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z46" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA46" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA46" t="inlineStr">
+      <c r="AB46" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB46" t="n">
+      <c r="AC46" t="n">
         <v>1</v>
       </c>
-      <c r="AC46" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD46" t="inlineStr">
+      <c r="AD46" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE46" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE46" t="inlineStr"/>
-      <c r="AF46" t="n">
+      <c r="AF46" t="inlineStr"/>
+      <c r="AG46" t="n">
         <v>13</v>
       </c>
-      <c r="AG46" t="inlineStr"/>
-      <c r="AH46" t="inlineStr">
+      <c r="AH46" t="inlineStr"/>
+      <c r="AI46" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI46" t="inlineStr">
+      <c r="AJ46" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -7244,41 +7474,46 @@
       <c r="X47" t="n">
         <v>101</v>
       </c>
-      <c r="Y47" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z47" t="inlineStr">
+      <c r="Y47" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z47" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA47" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA47" t="inlineStr">
+      <c r="AB47" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB47" t="n">
+      <c r="AC47" t="n">
         <v>1</v>
       </c>
-      <c r="AC47" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD47" t="inlineStr">
+      <c r="AD47" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE47" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE47" t="inlineStr"/>
-      <c r="AF47" t="n">
+      <c r="AF47" t="inlineStr"/>
+      <c r="AG47" t="n">
         <v>13</v>
       </c>
-      <c r="AG47" t="inlineStr"/>
-      <c r="AH47" t="inlineStr">
+      <c r="AH47" t="inlineStr"/>
+      <c r="AI47" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI47" t="inlineStr">
+      <c r="AJ47" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -7387,41 +7622,46 @@
       <c r="X48" t="n">
         <v>72</v>
       </c>
-      <c r="Y48" t="n">
+      <c r="Y48" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z48" t="n">
         <v>5</v>
       </c>
-      <c r="Z48" t="inlineStr">
+      <c r="AA48" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA48" t="inlineStr">
+      <c r="AB48" t="inlineStr">
         <is>
           <t>9, 10</t>
         </is>
       </c>
-      <c r="AB48" t="n">
+      <c r="AC48" t="n">
         <v>1</v>
       </c>
-      <c r="AC48" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD48" t="inlineStr">
+      <c r="AD48" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE48" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE48" t="inlineStr"/>
-      <c r="AF48" t="n">
-        <v>4</v>
-      </c>
-      <c r="AG48" t="inlineStr"/>
-      <c r="AH48" t="inlineStr">
+      <c r="AF48" t="inlineStr"/>
+      <c r="AG48" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH48" t="inlineStr"/>
+      <c r="AI48" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI48" t="inlineStr">
+      <c r="AJ48" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -7530,41 +7770,46 @@
       <c r="X49" t="n">
         <v>72</v>
       </c>
-      <c r="Y49" t="n">
+      <c r="Y49" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z49" t="n">
         <v>5</v>
       </c>
-      <c r="Z49" t="inlineStr">
+      <c r="AA49" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA49" t="inlineStr">
+      <c r="AB49" t="inlineStr">
         <is>
           <t>9, 10</t>
         </is>
       </c>
-      <c r="AB49" t="n">
+      <c r="AC49" t="n">
         <v>1</v>
       </c>
-      <c r="AC49" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD49" t="inlineStr">
+      <c r="AD49" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE49" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE49" t="inlineStr"/>
-      <c r="AF49" t="n">
-        <v>4</v>
-      </c>
-      <c r="AG49" t="inlineStr"/>
-      <c r="AH49" t="inlineStr">
+      <c r="AF49" t="inlineStr"/>
+      <c r="AG49" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH49" t="inlineStr"/>
+      <c r="AI49" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI49" t="inlineStr">
+      <c r="AJ49" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -7673,41 +7918,46 @@
       <c r="X50" t="n">
         <v>72</v>
       </c>
-      <c r="Y50" t="n">
+      <c r="Y50" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z50" t="n">
         <v>5</v>
       </c>
-      <c r="Z50" t="inlineStr">
+      <c r="AA50" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA50" t="inlineStr">
+      <c r="AB50" t="inlineStr">
         <is>
           <t>9, 10</t>
         </is>
       </c>
-      <c r="AB50" t="n">
+      <c r="AC50" t="n">
         <v>1</v>
       </c>
-      <c r="AC50" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD50" t="inlineStr">
+      <c r="AD50" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE50" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE50" t="inlineStr"/>
-      <c r="AF50" t="n">
-        <v>4</v>
-      </c>
-      <c r="AG50" t="inlineStr"/>
-      <c r="AH50" t="inlineStr">
+      <c r="AF50" t="inlineStr"/>
+      <c r="AG50" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH50" t="inlineStr"/>
+      <c r="AI50" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI50" t="inlineStr">
+      <c r="AJ50" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -7816,41 +8066,46 @@
       <c r="X51" t="n">
         <v>101</v>
       </c>
-      <c r="Y51" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z51" t="inlineStr">
+      <c r="Y51" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z51" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA51" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA51" t="inlineStr">
+      <c r="AB51" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB51" t="n">
+      <c r="AC51" t="n">
         <v>1</v>
       </c>
-      <c r="AC51" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD51" t="inlineStr">
+      <c r="AD51" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE51" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE51" t="inlineStr"/>
-      <c r="AF51" t="n">
+      <c r="AF51" t="inlineStr"/>
+      <c r="AG51" t="n">
         <v>13</v>
       </c>
-      <c r="AG51" t="inlineStr"/>
-      <c r="AH51" t="inlineStr">
+      <c r="AH51" t="inlineStr"/>
+      <c r="AI51" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI51" t="inlineStr">
+      <c r="AJ51" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -7963,41 +8218,46 @@
       <c r="X52" t="n">
         <v>400</v>
       </c>
-      <c r="Y52" t="n">
+      <c r="Y52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z52" t="n">
         <v>1</v>
       </c>
-      <c r="Z52" t="inlineStr">
+      <c r="AA52" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA52" t="inlineStr">
+      <c r="AB52" t="inlineStr">
         <is>
           <t>11, 12</t>
         </is>
       </c>
-      <c r="AB52" t="n">
+      <c r="AC52" t="n">
         <v>1</v>
       </c>
-      <c r="AC52" t="n">
+      <c r="AD52" t="n">
         <v>11</v>
       </c>
-      <c r="AD52" t="inlineStr">
+      <c r="AE52" t="inlineStr">
         <is>
           <t>MATH08051_lec</t>
         </is>
       </c>
-      <c r="AE52" t="inlineStr"/>
-      <c r="AF52" t="n">
+      <c r="AF52" t="inlineStr"/>
+      <c r="AG52" t="n">
         <v>1</v>
       </c>
-      <c r="AG52" t="inlineStr"/>
-      <c r="AH52" t="inlineStr">
+      <c r="AH52" t="inlineStr"/>
+      <c r="AI52" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI52" t="inlineStr">
+      <c r="AJ52" t="inlineStr">
         <is>
           <t>1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1</t>
         </is>
@@ -8110,41 +8370,46 @@
       <c r="X53" t="n">
         <v>400</v>
       </c>
-      <c r="Y53" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z53" t="inlineStr">
+      <c r="Y53" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z53" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA53" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA53" t="inlineStr">
+      <c r="AB53" t="inlineStr">
         <is>
           <t>11, 12</t>
         </is>
       </c>
-      <c r="AB53" t="n">
+      <c r="AC53" t="n">
         <v>1</v>
       </c>
-      <c r="AC53" t="n">
+      <c r="AD53" t="n">
         <v>11</v>
       </c>
-      <c r="AD53" t="inlineStr">
+      <c r="AE53" t="inlineStr">
         <is>
           <t>MATH08051_lec</t>
         </is>
       </c>
-      <c r="AE53" t="inlineStr"/>
-      <c r="AF53" t="n">
+      <c r="AF53" t="inlineStr"/>
+      <c r="AG53" t="n">
         <v>1</v>
       </c>
-      <c r="AG53" t="inlineStr"/>
-      <c r="AH53" t="inlineStr">
+      <c r="AH53" t="inlineStr"/>
+      <c r="AI53" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI53" t="inlineStr">
+      <c r="AJ53" t="inlineStr">
         <is>
           <t>1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1</t>
         </is>
@@ -8257,41 +8522,46 @@
       <c r="X54" t="n">
         <v>132</v>
       </c>
-      <c r="Y54" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z54" t="inlineStr">
+      <c r="Y54" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z54" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA54" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA54" t="inlineStr">
+      <c r="AB54" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB54" t="n">
+      <c r="AC54" t="n">
         <v>1</v>
       </c>
-      <c r="AC54" t="n">
+      <c r="AD54" t="n">
         <v>5</v>
       </c>
-      <c r="AD54" t="inlineStr">
+      <c r="AE54" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE54" t="inlineStr"/>
-      <c r="AF54" t="n">
+      <c r="AF54" t="inlineStr"/>
+      <c r="AG54" t="n">
         <v>9</v>
       </c>
-      <c r="AG54" t="inlineStr"/>
-      <c r="AH54" t="inlineStr">
+      <c r="AH54" t="inlineStr"/>
+      <c r="AI54" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI54" t="inlineStr">
+      <c r="AJ54" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -8404,41 +8674,46 @@
       <c r="X55" t="n">
         <v>132</v>
       </c>
-      <c r="Y55" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z55" t="inlineStr">
+      <c r="Y55" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA55" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA55" t="inlineStr">
+      <c r="AB55" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB55" t="n">
+      <c r="AC55" t="n">
         <v>1</v>
       </c>
-      <c r="AC55" t="n">
+      <c r="AD55" t="n">
         <v>5</v>
       </c>
-      <c r="AD55" t="inlineStr">
+      <c r="AE55" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE55" t="inlineStr"/>
-      <c r="AF55" t="n">
+      <c r="AF55" t="inlineStr"/>
+      <c r="AG55" t="n">
         <v>9</v>
       </c>
-      <c r="AG55" t="inlineStr"/>
-      <c r="AH55" t="inlineStr">
+      <c r="AH55" t="inlineStr"/>
+      <c r="AI55" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI55" t="inlineStr">
+      <c r="AJ55" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -8551,41 +8826,46 @@
       <c r="X56" t="n">
         <v>72</v>
       </c>
-      <c r="Y56" t="n">
+      <c r="Y56" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z56" t="n">
         <v>5</v>
       </c>
-      <c r="Z56" t="inlineStr">
+      <c r="AA56" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA56" t="inlineStr">
+      <c r="AB56" t="inlineStr">
         <is>
           <t>3, 4</t>
         </is>
       </c>
-      <c r="AB56" t="n">
+      <c r="AC56" t="n">
         <v>1</v>
       </c>
-      <c r="AC56" t="n">
+      <c r="AD56" t="n">
         <v>5</v>
       </c>
-      <c r="AD56" t="inlineStr">
+      <c r="AE56" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE56" t="inlineStr"/>
-      <c r="AF56" t="n">
+      <c r="AF56" t="inlineStr"/>
+      <c r="AG56" t="n">
         <v>5</v>
       </c>
-      <c r="AG56" t="inlineStr"/>
-      <c r="AH56" t="inlineStr">
+      <c r="AH56" t="inlineStr"/>
+      <c r="AI56" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI56" t="inlineStr">
+      <c r="AJ56" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -8698,41 +8978,46 @@
       <c r="X57" t="n">
         <v>72</v>
       </c>
-      <c r="Y57" t="n">
+      <c r="Y57" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z57" t="n">
         <v>5</v>
       </c>
-      <c r="Z57" t="inlineStr">
+      <c r="AA57" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA57" t="inlineStr">
+      <c r="AB57" t="inlineStr">
         <is>
           <t>5, 6</t>
         </is>
       </c>
-      <c r="AB57" t="n">
+      <c r="AC57" t="n">
         <v>1</v>
       </c>
-      <c r="AC57" t="n">
+      <c r="AD57" t="n">
         <v>5</v>
       </c>
-      <c r="AD57" t="inlineStr">
+      <c r="AE57" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE57" t="inlineStr"/>
-      <c r="AF57" t="n">
+      <c r="AF57" t="inlineStr"/>
+      <c r="AG57" t="n">
         <v>5</v>
       </c>
-      <c r="AG57" t="inlineStr"/>
-      <c r="AH57" t="inlineStr">
+      <c r="AH57" t="inlineStr"/>
+      <c r="AI57" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI57" t="inlineStr">
+      <c r="AJ57" t="inlineStr">
         <is>
           <t>0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1</t>
         </is>
@@ -8841,41 +9126,46 @@
       <c r="X58" t="n">
         <v>132</v>
       </c>
-      <c r="Y58" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z58" t="inlineStr">
+      <c r="Y58" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z58" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA58" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA58" t="inlineStr">
+      <c r="AB58" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB58" t="n">
+      <c r="AC58" t="n">
         <v>1</v>
       </c>
-      <c r="AC58" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD58" t="inlineStr">
+      <c r="AD58" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE58" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE58" t="inlineStr"/>
-      <c r="AF58" t="n">
+      <c r="AF58" t="inlineStr"/>
+      <c r="AG58" t="n">
         <v>14</v>
       </c>
-      <c r="AG58" t="inlineStr"/>
-      <c r="AH58" t="inlineStr">
+      <c r="AH58" t="inlineStr"/>
+      <c r="AI58" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI58" t="inlineStr">
+      <c r="AJ58" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -8984,41 +9274,46 @@
       <c r="X59" t="n">
         <v>101</v>
       </c>
-      <c r="Y59" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z59" t="inlineStr">
+      <c r="Y59" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z59" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA59" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA59" t="inlineStr">
+      <c r="AB59" t="inlineStr">
         <is>
           <t>13, 14</t>
         </is>
       </c>
-      <c r="AB59" t="n">
+      <c r="AC59" t="n">
         <v>1</v>
       </c>
-      <c r="AC59" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD59" t="inlineStr">
+      <c r="AD59" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE59" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE59" t="inlineStr"/>
-      <c r="AF59" t="n">
+      <c r="AF59" t="inlineStr"/>
+      <c r="AG59" t="n">
         <v>14</v>
       </c>
-      <c r="AG59" t="inlineStr"/>
-      <c r="AH59" t="inlineStr">
+      <c r="AH59" t="inlineStr"/>
+      <c r="AI59" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI59" t="inlineStr">
+      <c r="AJ59" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -9127,41 +9422,46 @@
       <c r="X60" t="n">
         <v>132</v>
       </c>
-      <c r="Y60" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z60" t="inlineStr">
+      <c r="Y60" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z60" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA60" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA60" t="inlineStr">
+      <c r="AB60" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB60" t="n">
+      <c r="AC60" t="n">
         <v>1</v>
       </c>
-      <c r="AC60" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD60" t="inlineStr">
+      <c r="AD60" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE60" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE60" t="inlineStr"/>
-      <c r="AF60" t="n">
+      <c r="AF60" t="inlineStr"/>
+      <c r="AG60" t="n">
         <v>13</v>
       </c>
-      <c r="AG60" t="inlineStr"/>
-      <c r="AH60" t="inlineStr">
+      <c r="AH60" t="inlineStr"/>
+      <c r="AI60" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI60" t="inlineStr">
+      <c r="AJ60" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -9270,41 +9570,46 @@
       <c r="X61" t="n">
         <v>101</v>
       </c>
-      <c r="Y61" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z61" t="inlineStr">
+      <c r="Y61" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z61" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA61" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA61" t="inlineStr">
+      <c r="AB61" t="inlineStr">
         <is>
           <t>15, 16</t>
         </is>
       </c>
-      <c r="AB61" t="n">
+      <c r="AC61" t="n">
         <v>1</v>
       </c>
-      <c r="AC61" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD61" t="inlineStr">
+      <c r="AD61" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE61" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE61" t="inlineStr"/>
-      <c r="AF61" t="n">
+      <c r="AF61" t="inlineStr"/>
+      <c r="AG61" t="n">
         <v>13</v>
       </c>
-      <c r="AG61" t="inlineStr"/>
-      <c r="AH61" t="inlineStr">
+      <c r="AH61" t="inlineStr"/>
+      <c r="AI61" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI61" t="inlineStr">
+      <c r="AJ61" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>
@@ -9413,41 +9718,46 @@
       <c r="X62" t="n">
         <v>72</v>
       </c>
-      <c r="Y62" t="n">
+      <c r="Y62" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z62" t="n">
         <v>5</v>
       </c>
-      <c r="Z62" t="inlineStr">
+      <c r="AA62" t="inlineStr">
         <is>
           <t>SY2</t>
         </is>
       </c>
-      <c r="AA62" t="inlineStr">
+      <c r="AB62" t="inlineStr">
         <is>
           <t>9, 10</t>
         </is>
       </c>
-      <c r="AB62" t="n">
+      <c r="AC62" t="n">
         <v>1</v>
       </c>
-      <c r="AC62" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD62" t="inlineStr">
+      <c r="AD62" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE62" t="inlineStr">
         <is>
           <t>MATH08051_ws</t>
         </is>
       </c>
-      <c r="AE62" t="inlineStr"/>
-      <c r="AF62" t="n">
-        <v>4</v>
-      </c>
-      <c r="AG62" t="inlineStr"/>
-      <c r="AH62" t="inlineStr">
+      <c r="AF62" t="inlineStr"/>
+      <c r="AG62" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH62" t="inlineStr"/>
+      <c r="AI62" t="inlineStr">
         <is>
           <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0</t>
         </is>
       </c>
-      <c r="AI62" t="inlineStr">
+      <c r="AJ62" t="inlineStr">
         <is>
           <t>0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0</t>
         </is>

</xml_diff>